<commit_message>
Change to memory grav
</commit_message>
<xml_diff>
--- a/pendulum/random_mem_grav/random_mem_grav.xlsx
+++ b/pendulum/random_mem_grav/random_mem_grav.xlsx
@@ -3,11 +3,12 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15800" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="17" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="18" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="181029" fullCalcOnLoad="1"/>
@@ -792,4 +793,518 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(cos(cos(0)), sub(sin(sin(sin(sin(read(a0, a2))))), write(a0, abs(0), a2)))</t>
+        </is>
+      </c>
+      <c r="B1" t="n">
+        <v>-53.31</v>
+      </c>
+      <c r="C1" t="n">
+        <v>-57.58</v>
+      </c>
+      <c r="D1" t="n">
+        <v>-102.85</v>
+      </c>
+      <c r="E1" t="n">
+        <v>-583.55</v>
+      </c>
+      <c r="F1" t="n">
+        <v>-590.15</v>
+      </c>
+      <c r="G1" t="n">
+        <v>-540</v>
+      </c>
+      <c r="H1" t="n">
+        <v>-460</v>
+      </c>
+      <c r="I1" t="n">
+        <v>-372.36</v>
+      </c>
+      <c r="J1" t="n">
+        <v>-297.4</v>
+      </c>
+      <c r="K1" t="n">
+        <v>-347.22</v>
+      </c>
+      <c r="L1" t="n">
+        <v>-321.09</v>
+      </c>
+      <c r="M1" t="n">
+        <v>-664.26</v>
+      </c>
+      <c r="N1" t="n">
+        <v>-766.38</v>
+      </c>
+      <c r="O1" t="n">
+        <v>-1101.66</v>
+      </c>
+      <c r="P1" t="n">
+        <v>-1474.13</v>
+      </c>
+      <c r="Q1" t="n">
+        <v>-1690.89</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(memProtectedDiv(a2, conditional(sin(a1), 0)), protectedLog(cos(write(a0, a2, sin(sin(add(read(a0, 0), a2)))))))</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-298.07</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-268.19</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-179.47</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-200.48</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-856.99</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-796.25</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-816.22</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-918.39</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1041.32</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-1206.02</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1225.25</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-1296.17</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1394</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-1396.53</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-1378.41</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-1731.88</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(add(add(a2, a2), read(a0, a1)), conditional(sin(sin(sin(sin(read(a0, cos(protectedLog(memProtectedDiv(a1, a2)))))))), write(a0, limit(sub(a1, a1), protectedLog(conditional(sin(sin(read(a0, 0))), write(a0, sin(add(a2, a2)), sub(protectedLog(read(a0, 0)), write(a0, 0, cos(conditional(a1, a2))))))), a1), a2)))</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-88.03</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-76.05</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-68.04000000000001</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-129.26</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-651.55</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-547.71</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-427.1</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-376.66</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-414.86</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-387.87</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-434.88</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-796.75</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-969.4</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-1125.85</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-1421.98</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-1678.01</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>sub(sub(sub(read(a0, 0), memProtectedDiv(a2, abs(read(a0, sub(cos(protectedLog(add(0, a1))), a1))))), write(a0, sin(read(a0, memProtectedDiv(a2, a1))), a2)), a2)</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>-157.45</v>
+      </c>
+      <c r="C4" t="n">
+        <v>-122.33</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-110.08</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-182.15</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-675.09</v>
+      </c>
+      <c r="G4" t="n">
+        <v>-771.4400000000001</v>
+      </c>
+      <c r="H4" t="n">
+        <v>-846.36</v>
+      </c>
+      <c r="I4" t="n">
+        <v>-894.27</v>
+      </c>
+      <c r="J4" t="n">
+        <v>-1034.44</v>
+      </c>
+      <c r="K4" t="n">
+        <v>-1097.06</v>
+      </c>
+      <c r="L4" t="n">
+        <v>-1186.2</v>
+      </c>
+      <c r="M4" t="n">
+        <v>-1255.08</v>
+      </c>
+      <c r="N4" t="n">
+        <v>-1269.79</v>
+      </c>
+      <c r="O4" t="n">
+        <v>-1316.21</v>
+      </c>
+      <c r="P4" t="n">
+        <v>-1345.97</v>
+      </c>
+      <c r="Q4" t="n">
+        <v>-1634.54</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>memProtectedDiv(sub(write(a0, a1, sub(sub(sub(read(a0, 0), a2), a2), abs(protectedLog(0)))), write(a0, conditional(cos(a1), a1), add(write(a0, a1, add(write(a0, a1, add(a2, add(0, a2))), add(limit(a2, 0, write(a0, a1, 0)), a2))), a2))), abs(a2))</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>-63.25</v>
+      </c>
+      <c r="C5" t="n">
+        <v>-63.72</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-58.33</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-106.62</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-371.9</v>
+      </c>
+      <c r="G5" t="n">
+        <v>-386.74</v>
+      </c>
+      <c r="H5" t="n">
+        <v>-493.96</v>
+      </c>
+      <c r="I5" t="n">
+        <v>-638.3200000000001</v>
+      </c>
+      <c r="J5" t="n">
+        <v>-870.0700000000001</v>
+      </c>
+      <c r="K5" t="n">
+        <v>-844.96</v>
+      </c>
+      <c r="L5" t="n">
+        <v>-982.09</v>
+      </c>
+      <c r="M5" t="n">
+        <v>-957.25</v>
+      </c>
+      <c r="N5" t="n">
+        <v>-928.6799999999999</v>
+      </c>
+      <c r="O5" t="n">
+        <v>-355.68</v>
+      </c>
+      <c r="P5" t="n">
+        <v>-616.05</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>-1483.02</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>sub(sub(0, memProtectedDiv(conditional(a2, read(a0, a2)), write(a0, 0, sin(a2)))), memProtectedDiv(conditional(read(a0, 0), 0), a2))</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>-68.2</v>
+      </c>
+      <c r="C6" t="n">
+        <v>-77.67</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-68.23</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-101.44</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-422.63</v>
+      </c>
+      <c r="G6" t="n">
+        <v>-382.93</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-373.76</v>
+      </c>
+      <c r="I6" t="n">
+        <v>-365.42</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-487.3</v>
+      </c>
+      <c r="K6" t="n">
+        <v>-624.72</v>
+      </c>
+      <c r="L6" t="n">
+        <v>-714.51</v>
+      </c>
+      <c r="M6" t="n">
+        <v>-789.6799999999999</v>
+      </c>
+      <c r="N6" t="n">
+        <v>-771.95</v>
+      </c>
+      <c r="O6" t="n">
+        <v>-594</v>
+      </c>
+      <c r="P6" t="n">
+        <v>-1362.07</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>-1493.48</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sub(sub(sub(sub(read(a0, add(add(memProtectedDiv(0, 0), a1), a1)), write(a0, limit(0, sub(add(0, a2), protectedLog(a1)), abs(a2)), add(add(memProtectedDiv(protectedLog(abs(a2)), sin(a2)), memProtectedDiv(a1, conditional(a2, a1))), a2))), sin(read(a0, add(read(a0, a2), a2)))), a2), add(a2, a2))</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>-87.09</v>
+      </c>
+      <c r="C7" t="n">
+        <v>-88.98999999999999</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-84.65000000000001</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-189.07</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-210.36</v>
+      </c>
+      <c r="G7" t="n">
+        <v>-219.76</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-246.34</v>
+      </c>
+      <c r="I7" t="n">
+        <v>-244.69</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-338.3</v>
+      </c>
+      <c r="K7" t="n">
+        <v>-422.06</v>
+      </c>
+      <c r="L7" t="n">
+        <v>-457.37</v>
+      </c>
+      <c r="M7" t="n">
+        <v>-538.99</v>
+      </c>
+      <c r="N7" t="n">
+        <v>-921.0700000000001</v>
+      </c>
+      <c r="O7" t="n">
+        <v>-1432.88</v>
+      </c>
+      <c r="P7" t="n">
+        <v>-1572.6</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>-1684.28</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a2), memProtectedDiv(abs(memProtectedDiv(memProtectedDiv(write(a0, protectedLog(0), add(a2, a2)), a1), a1)), a2))</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>-254.59</v>
+      </c>
+      <c r="C8" t="n">
+        <v>-305.07</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-251.89</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-306.78</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-803.49</v>
+      </c>
+      <c r="G8" t="n">
+        <v>-902.97</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-1105.06</v>
+      </c>
+      <c r="I8" t="n">
+        <v>-1204.28</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-1313.37</v>
+      </c>
+      <c r="K8" t="n">
+        <v>-1460.39</v>
+      </c>
+      <c r="L8" t="n">
+        <v>-1477.73</v>
+      </c>
+      <c r="M8" t="n">
+        <v>-1497.64</v>
+      </c>
+      <c r="N8" t="n">
+        <v>-1543.71</v>
+      </c>
+      <c r="O8" t="n">
+        <v>-1529.84</v>
+      </c>
+      <c r="P8" t="n">
+        <v>-1460.22</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>-1714.57</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>sub(read(a0, a2), add(a2, add(add(a2, write(a0, sin(a1), sub(a1, memProtectedDiv(conditional(memProtectedDiv(a1, a2), a2), a2)))), add(a2, cos(read(a0, 0))))))</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>-99.48999999999999</v>
+      </c>
+      <c r="C9" t="n">
+        <v>-92.16</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-97.34</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-180.29</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-194.12</v>
+      </c>
+      <c r="G9" t="n">
+        <v>-205.33</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-251.55</v>
+      </c>
+      <c r="I9" t="n">
+        <v>-278.61</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-351.4</v>
+      </c>
+      <c r="K9" t="n">
+        <v>-402.72</v>
+      </c>
+      <c r="L9" t="n">
+        <v>-483.8</v>
+      </c>
+      <c r="M9" t="n">
+        <v>-627.42</v>
+      </c>
+      <c r="N9" t="n">
+        <v>-1101.22</v>
+      </c>
+      <c r="O9" t="n">
+        <v>-1375.39</v>
+      </c>
+      <c r="P9" t="n">
+        <v>-1565.57</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>-1757.59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
apply changes to random full grav
</commit_message>
<xml_diff>
--- a/pendulum/random_mem_grav/random_mem_grav.xlsx
+++ b/pendulum/random_mem_grav/random_mem_grav.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sky/Documents/Work Info/Research Assistant/deap_experiments/pendulum/random_mem_grav/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34AE49D9-3D5B-514F-B49D-A12ADF3B75A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4920D44F-0308-2947-8149-4C827E75E1F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="15660" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="13" sheetId="3" r:id="rId1"/>
+    <sheet name="13 (old)" sheetId="1" r:id="rId1"/>
+    <sheet name="13" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+  <si>
+    <t>Ind</t>
+  </si>
   <si>
     <t>memProtectedDiv(cos(cos(0)), sub(sin(sin(sin(sin(read(a0, a2))))), write(a0, abs(0), a2)))</t>
   </si>
@@ -62,10 +66,43 @@
     <t>sub(read(a0, a2), add(a2, add(add(a2, write(a0, sin(a1), sub(a1, memProtectedDiv(conditional(memProtectedDiv(a1, a2), a2), a2)))), add(a2, cos(read(a0, 0))))))</t>
   </si>
   <si>
-    <t>Ind</t>
+    <t>Fit</t>
   </si>
   <si>
-    <t>Fit</t>
+    <t>sub(sub(sub(sub(sub(sub(sub(sub(sub(write(a0, a1, sin(add(read(a0, cos(protectedLog(abs(abs(a1))))), a2))), a2), memProtectedDiv(0, limit(abs(cos(0)), a2, sin(0)))), sin(a2)), a2), a2), a2), a2), a2), a2)</t>
+  </si>
+  <si>
+    <t>sub(read(a0, a1), add(add(a2, sin(read(a0, abs(0)))), add(add(a2, a2), write(a0, 0, add(a2, memProtectedDiv(sub(write(a0, a1, 0), conditional(add(sub(a1, 0), add(a1, a1)), read(a0, a2))), a2))))))</t>
+  </si>
+  <si>
+    <t>sub(sub(sub(read(a0, a1), a2), add(a2, write(a0, write(a0, 0, 0), add(0, add(memProtectedDiv(protectedLog(cos(a1)), a2), write(a0, limit(limit(a2, add(conditional(abs(a1), 0), 0), abs(sub(memProtectedDiv(sub(a2, a1), a2), write(a0, 0, write(a0, a2, a1))))), 0, a2), add(add(add(a2, add(a2, write(a0, 0, add(add(write(a0, sin(a2), a2), a2), a2)))), 0), write(a0, abs(cos(a2)), add(a2, read(a0, 0)))))))))), sin(read(a0, a1)))</t>
+  </si>
+  <si>
+    <t>sub(sub(0, memProtectedDiv(cos(limit(cos(0), memProtectedDiv(read(a0, 0), write(a0, add(protectedLog(cos(limit(abs(a1), 0, a1))), a1), protectedLog(abs(conditional(a1, sin(0)))))), a1)), a2)), a2)</t>
+  </si>
+  <si>
+    <t>sub(read(a0, 0), add(add(add(write(a0, 0, memProtectedDiv(protectedLog(abs(write(a0, sub(conditional(add(a2, a2), conditional(0, a2)), cos(0)), protectedLog(abs(a1))))), a2)), a2), add(sin(read(a0, a1)), a2)), a2))</t>
+  </si>
+  <si>
+    <t>sub(sub(0, a2), memProtectedDiv(conditional(add(conditional(read(a0, a1), a1), cos(protectedLog(write(a0, sin(memProtectedDiv(0, protectedLog(a2))), a1)))), abs(a1)), a2))</t>
+  </si>
+  <si>
+    <t>sub(memProtectedDiv(a2, sub(0, cos(a1))), memProtectedDiv(cos(memProtectedDiv(read(a0, sub(a1, a2)), a2)), write(a0, a1, memProtectedDiv(a2, read(a0, write(a0, a1, sin(memProtectedDiv(a1, a1))))))))</t>
+  </si>
+  <si>
+    <t>sub(0, add(memProtectedDiv(write(a0, abs(write(a0, a1, sin(read(a0, conditional(0, 0))))), conditional(abs(a2), read(a0, a1))), sin(a2)), memProtectedDiv(write(a0, cos(a2), conditional(a2, sin(0))), a2)))</t>
+  </si>
+  <si>
+    <t>sub(read(a0, abs(a1)), add(add(sin(read(a0, write(a0, a2, add(0, sub(sub(0, memProtectedDiv(cos(a2), a2)), memProtectedDiv(abs(cos(memProtectedDiv(0, sub(a2, sin(write(a0, 0, sin(cos(a2)))))))), a2)))))), add(a2, a2)), add(a2, write(a0, memProtectedDiv(a1, a2), add(add(a2, sub(conditional(a1, protectedLog(a2)), memProtectedDiv(cos(a2), a2))), sub(write(a0, 0, add(a1, sub(a2, memProtectedDiv(cos(0), a2)))), memProtectedDiv(cos(0), a2)))))))</t>
+  </si>
+  <si>
+    <t>sub(sub(sub(read(a0, sin(a1)), a2), write(a0, a1, sub(a2, memProtectedDiv(conditional(memProtectedDiv(a1, a2), a2), a2)))), memProtectedDiv(cos(cos(0)), a2))</t>
+  </si>
+  <si>
+    <t>sub(add(read(a0, add(a1, 0)), sub(sub(0, write(a0, a1, add(a2, write(a0, limit(memProtectedDiv(abs(sub(write(a0, 0, a1), a1)), 0), a1, conditional(conditional(limit(sub(a2, protectedLog(0)), 0, sin(a2)), write(a0, 0, a1)), read(a0, cos(a2)))), add(add(memProtectedDiv(sub(sub(protectedLog(a1), a1), a1), memProtectedDiv(a2, a1)), add(write(a0, sin(a2), a2), a2)), a2))))), memProtectedDiv(abs(a2), a2))), a2)</t>
+  </si>
+  <si>
+    <t>sub(read(a0, a1), add(sin(read(a0, a1)), add(add(a2, add(write(a0, 0, add(a2, add(add(memProtectedDiv(a1, conditional(a2, a1)), a2), memProtectedDiv(a1, conditional(a2, a1))))), a2)), a2)))</t>
   </si>
 </sst>
 </file>
@@ -118,6 +155,1411 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'13'!$A$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Fit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'13'!$B$14:$Q$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>17</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'13'!$B$15:$Q$15</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>-80.944999999999993</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-78.33</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-90.335000000000008</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-207.785</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-219.01</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-238.595</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-278.23</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-317.53999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-359.07</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-424.98500000000001</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-478.76</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-559.53500000000008</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1045.5150000000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1393.3</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>-1584.2950000000001</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>-1706.6849999999999</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-4ABA-604A-9C20-7DD4D7FF4FC8}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="912720128"/>
+        <c:axId val="912728864"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="912720128"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="912728864"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="912728864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="912720128"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>418830</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>94574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>491787</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>17563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29B3403E-5ED0-D19A-4FCB-9C39FB71C6D6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="418830" y="3945106"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>702553</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>81064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>775511</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>4053</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D538B41C-F01F-73F9-FAA0-9E9A0CCF3D0B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6471596" y="3931596"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>337766</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>27022</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>410723</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>152671</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E821E70-A0C5-3841-D2FE-5F7117C963C5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12700000" y="3877554"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>378298</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>189148</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>451255</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>112138</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0110809F-54A7-A579-6755-0FA78748AB22}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="378298" y="8498191"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>702553</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>94574</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>775511</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>17563</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{86BE1ADD-42CC-B949-B05C-583A1C52E779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6471596" y="8606276"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>337765</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>13511</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>410722</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>139160</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F1E8B80-1469-D1AF-C157-8FBD23C54BDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12699999" y="8525213"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>310744</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>81064</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>383701</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>4053</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A01D8B0D-DC0A-806B-92DF-E4099206E12F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="310744" y="13253936"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>743084</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>40532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>816042</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>166181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56FCF252-52EB-4DF8-3E0F-D8D339745CF7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6512127" y="13213404"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>283723</xdr:colOff>
+      <xdr:row>65</xdr:row>
+      <xdr:rowOff>40532</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>356680</xdr:colOff>
+      <xdr:row>86</xdr:row>
+      <xdr:rowOff>166181</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{06DC533A-A9BE-296E-7B78-2EC561E52BBB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12645957" y="13213404"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D184EC0C-FB2B-EE6C-7615-F48ACBD1699A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19431000" y="3937000"/>
+          <a:ext cx="5842000" cy="4381500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>-1</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>334432</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="23" name="Chart 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFF35483-5B64-B671-DD72-F1DFE5D75B51}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -416,10 +1858,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
@@ -427,7 +1869,7 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="B1">
         <v>1</v>
@@ -480,7 +1922,7 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>-53.31</v>
@@ -533,7 +1975,7 @@
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>-298.07</v>
@@ -586,7 +2028,7 @@
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4">
         <v>-88.03</v>
@@ -639,7 +2081,7 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>-157.44999999999999</v>
@@ -692,7 +2134,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6">
         <v>-63.25</v>
@@ -745,7 +2187,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7">
         <v>-68.2</v>
@@ -798,7 +2240,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8">
         <v>-87.09</v>
@@ -851,7 +2293,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>-254.59</v>
@@ -904,7 +2346,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10">
         <v>-99.49</v>
@@ -1010,11 +2452,11 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <f>AVERAGE(B2:B10)</f>
+        <f t="shared" ref="B12:Q12" si="0">AVERAGE(B2:B10)</f>
         <v>-129.94222222222223</v>
       </c>
       <c r="C12">
-        <f t="shared" ref="C12:Q12" si="0">AVERAGE(C2:C10)</f>
+        <f t="shared" si="0"/>
         <v>-127.97333333333333</v>
       </c>
       <c r="D12">
@@ -1129,11 +2571,11 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <f>MEDIAN(B2:B10)</f>
+        <f t="shared" ref="B14:Q14" si="1">MEDIAN(B2:B10)</f>
         <v>-88.03</v>
       </c>
       <c r="C14">
-        <f t="shared" ref="C14:Q14" si="1">MEDIAN(C2:C10)</f>
+        <f t="shared" si="1"/>
         <v>-88.99</v>
       </c>
       <c r="D14">
@@ -1196,4 +2638,775 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:Q15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="50" workbookViewId="0">
+      <selection activeCell="AJ51" sqref="AJ51"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1">
+        <v>-261.82</v>
+      </c>
+      <c r="C1">
+        <v>-205.62</v>
+      </c>
+      <c r="D1">
+        <v>-174.18</v>
+      </c>
+      <c r="E1">
+        <v>-172.21</v>
+      </c>
+      <c r="F1">
+        <v>-745.77</v>
+      </c>
+      <c r="G1">
+        <v>-767.63</v>
+      </c>
+      <c r="H1">
+        <v>-825.81</v>
+      </c>
+      <c r="I1">
+        <v>-802.79</v>
+      </c>
+      <c r="J1">
+        <v>-1210.19</v>
+      </c>
+      <c r="K1">
+        <v>-1253.99</v>
+      </c>
+      <c r="L1">
+        <v>-1312.27</v>
+      </c>
+      <c r="M1">
+        <v>-1378.42</v>
+      </c>
+      <c r="N1">
+        <v>-1464.8</v>
+      </c>
+      <c r="O1">
+        <v>-1488.46</v>
+      </c>
+      <c r="P1">
+        <v>-1473.62</v>
+      </c>
+      <c r="Q1">
+        <v>-1708.91</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>-83.89</v>
+      </c>
+      <c r="C2">
+        <v>-64.44</v>
+      </c>
+      <c r="D2">
+        <v>-79.650000000000006</v>
+      </c>
+      <c r="E2">
+        <v>-181.46</v>
+      </c>
+      <c r="F2">
+        <v>-203.06</v>
+      </c>
+      <c r="G2">
+        <v>-228.78</v>
+      </c>
+      <c r="H2">
+        <v>-256.88</v>
+      </c>
+      <c r="I2">
+        <v>-289.43</v>
+      </c>
+      <c r="J2">
+        <v>-293.89999999999998</v>
+      </c>
+      <c r="K2">
+        <v>-387.92</v>
+      </c>
+      <c r="L2">
+        <v>-427.01</v>
+      </c>
+      <c r="M2">
+        <v>-513.55999999999995</v>
+      </c>
+      <c r="N2">
+        <v>-1163.42</v>
+      </c>
+      <c r="O2">
+        <v>-1397.56</v>
+      </c>
+      <c r="P2">
+        <v>-1620.53</v>
+      </c>
+      <c r="Q2">
+        <v>-1712.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>-72.510000000000005</v>
+      </c>
+      <c r="C3">
+        <v>-97.24</v>
+      </c>
+      <c r="D3">
+        <v>-148.68</v>
+      </c>
+      <c r="E3">
+        <v>-228.51</v>
+      </c>
+      <c r="F3">
+        <v>-206.8</v>
+      </c>
+      <c r="G3">
+        <v>-240.4</v>
+      </c>
+      <c r="H3">
+        <v>-296.66000000000003</v>
+      </c>
+      <c r="I3">
+        <v>-345.65</v>
+      </c>
+      <c r="J3">
+        <v>-434.75</v>
+      </c>
+      <c r="K3">
+        <v>-384.97</v>
+      </c>
+      <c r="L3">
+        <v>-449.64</v>
+      </c>
+      <c r="M3">
+        <v>-528.02</v>
+      </c>
+      <c r="N3">
+        <v>-1246.95</v>
+      </c>
+      <c r="O3">
+        <v>-1510.78</v>
+      </c>
+      <c r="P3">
+        <v>-1593.99</v>
+      </c>
+      <c r="Q3">
+        <v>-1701.65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>-64.78</v>
+      </c>
+      <c r="C4">
+        <v>-56.12</v>
+      </c>
+      <c r="D4">
+        <v>-82.95</v>
+      </c>
+      <c r="E4">
+        <v>-262.55</v>
+      </c>
+      <c r="F4">
+        <v>-248.56</v>
+      </c>
+      <c r="G4">
+        <v>-307.49</v>
+      </c>
+      <c r="H4">
+        <v>-341.89</v>
+      </c>
+      <c r="I4">
+        <v>-390.96</v>
+      </c>
+      <c r="J4">
+        <v>-394.95</v>
+      </c>
+      <c r="K4">
+        <v>-449.76</v>
+      </c>
+      <c r="L4">
+        <v>-447.65</v>
+      </c>
+      <c r="M4">
+        <v>-422.43</v>
+      </c>
+      <c r="N4">
+        <v>-397.36</v>
+      </c>
+      <c r="O4">
+        <v>-884.04</v>
+      </c>
+      <c r="P4">
+        <v>-1520.8</v>
+      </c>
+      <c r="Q4">
+        <v>-1656.59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>-79.650000000000006</v>
+      </c>
+      <c r="C5">
+        <v>-84.63</v>
+      </c>
+      <c r="D5">
+        <v>-89.99</v>
+      </c>
+      <c r="E5">
+        <v>-207.69</v>
+      </c>
+      <c r="F5">
+        <v>-200.68</v>
+      </c>
+      <c r="G5">
+        <v>-212.52</v>
+      </c>
+      <c r="H5">
+        <v>-225.48</v>
+      </c>
+      <c r="I5">
+        <v>-261.39999999999998</v>
+      </c>
+      <c r="J5">
+        <v>-335.59</v>
+      </c>
+      <c r="K5">
+        <v>-365.92</v>
+      </c>
+      <c r="L5">
+        <v>-503.08</v>
+      </c>
+      <c r="M5">
+        <v>-605.98</v>
+      </c>
+      <c r="N5">
+        <v>-1189.29</v>
+      </c>
+      <c r="O5">
+        <v>-1387.66</v>
+      </c>
+      <c r="P5">
+        <v>-1603.75</v>
+      </c>
+      <c r="Q5">
+        <v>-1704.46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>-124.3</v>
+      </c>
+      <c r="C6">
+        <v>-100.64</v>
+      </c>
+      <c r="D6">
+        <v>-256.77999999999997</v>
+      </c>
+      <c r="E6">
+        <v>-325.22000000000003</v>
+      </c>
+      <c r="F6">
+        <v>-222.88</v>
+      </c>
+      <c r="G6">
+        <v>-337.24</v>
+      </c>
+      <c r="H6">
+        <v>-347.76</v>
+      </c>
+      <c r="I6">
+        <v>-383.14</v>
+      </c>
+      <c r="J6">
+        <v>-646.61</v>
+      </c>
+      <c r="K6">
+        <v>-640.54999999999995</v>
+      </c>
+      <c r="L6">
+        <v>-757.76</v>
+      </c>
+      <c r="M6">
+        <v>-930.42</v>
+      </c>
+      <c r="N6">
+        <v>-961.13</v>
+      </c>
+      <c r="O6">
+        <v>-1369.77</v>
+      </c>
+      <c r="P6">
+        <v>-1573.8</v>
+      </c>
+      <c r="Q6">
+        <v>-1753.07</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>-82.24</v>
+      </c>
+      <c r="C7">
+        <v>-73.94</v>
+      </c>
+      <c r="D7">
+        <v>-311.12</v>
+      </c>
+      <c r="E7">
+        <v>-481.96</v>
+      </c>
+      <c r="F7">
+        <v>-498.83</v>
+      </c>
+      <c r="G7">
+        <v>-526.21</v>
+      </c>
+      <c r="H7">
+        <v>-592.96</v>
+      </c>
+      <c r="I7">
+        <v>-587.63</v>
+      </c>
+      <c r="J7">
+        <v>-603.73</v>
+      </c>
+      <c r="K7">
+        <v>-704.13</v>
+      </c>
+      <c r="L7">
+        <v>-654.01</v>
+      </c>
+      <c r="M7">
+        <v>-662.51</v>
+      </c>
+      <c r="N7">
+        <v>-639.94000000000005</v>
+      </c>
+      <c r="O7">
+        <v>-718.69</v>
+      </c>
+      <c r="P7">
+        <v>-1504.48</v>
+      </c>
+      <c r="Q7">
+        <v>-1619.79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8">
+        <v>-79.180000000000007</v>
+      </c>
+      <c r="C8">
+        <v>-85.97</v>
+      </c>
+      <c r="D8">
+        <v>-71.97</v>
+      </c>
+      <c r="E8">
+        <v>-106.19</v>
+      </c>
+      <c r="F8">
+        <v>-488.95</v>
+      </c>
+      <c r="G8">
+        <v>-338.77</v>
+      </c>
+      <c r="H8">
+        <v>-298.52999999999997</v>
+      </c>
+      <c r="I8">
+        <v>-350.88</v>
+      </c>
+      <c r="J8">
+        <v>-357.36</v>
+      </c>
+      <c r="K8">
+        <v>-439.75</v>
+      </c>
+      <c r="L8">
+        <v>-541.46</v>
+      </c>
+      <c r="M8">
+        <v>-622.84</v>
+      </c>
+      <c r="N8">
+        <v>-793.75</v>
+      </c>
+      <c r="O8">
+        <v>-660.19</v>
+      </c>
+      <c r="P8">
+        <v>-1439.64</v>
+      </c>
+      <c r="Q8">
+        <v>-1536.79</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9">
+        <v>-96.05</v>
+      </c>
+      <c r="C9">
+        <v>-82.69</v>
+      </c>
+      <c r="D9">
+        <v>-88.46</v>
+      </c>
+      <c r="E9">
+        <v>-244.31</v>
+      </c>
+      <c r="F9">
+        <v>-215.14</v>
+      </c>
+      <c r="G9">
+        <v>-212.83</v>
+      </c>
+      <c r="H9">
+        <v>-259.8</v>
+      </c>
+      <c r="I9">
+        <v>-286.77</v>
+      </c>
+      <c r="J9">
+        <v>-345.32</v>
+      </c>
+      <c r="K9">
+        <v>-458.16</v>
+      </c>
+      <c r="L9">
+        <v>-484.45</v>
+      </c>
+      <c r="M9">
+        <v>-561.57000000000005</v>
+      </c>
+      <c r="N9">
+        <v>-947.98</v>
+      </c>
+      <c r="O9">
+        <v>-1389.04</v>
+      </c>
+      <c r="P9">
+        <v>-1614.95</v>
+      </c>
+      <c r="Q9">
+        <v>-1728.51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10">
+        <v>-88.3</v>
+      </c>
+      <c r="C10">
+        <v>-68.510000000000005</v>
+      </c>
+      <c r="D10">
+        <v>-94.32</v>
+      </c>
+      <c r="E10">
+        <v>-207.88</v>
+      </c>
+      <c r="F10">
+        <v>-188.69</v>
+      </c>
+      <c r="G10">
+        <v>-216.55</v>
+      </c>
+      <c r="H10">
+        <v>-232.06</v>
+      </c>
+      <c r="I10">
+        <v>-250.84</v>
+      </c>
+      <c r="J10">
+        <v>-300.38</v>
+      </c>
+      <c r="K10">
+        <v>-325</v>
+      </c>
+      <c r="L10">
+        <v>-357.31</v>
+      </c>
+      <c r="M10">
+        <v>-371.75</v>
+      </c>
+      <c r="N10">
+        <v>-693.77</v>
+      </c>
+      <c r="O10">
+        <v>-1475.91</v>
+      </c>
+      <c r="P10">
+        <v>-1598.52</v>
+      </c>
+      <c r="Q10">
+        <v>-1762.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11">
+        <v>-68.2</v>
+      </c>
+      <c r="C11">
+        <v>-62.47</v>
+      </c>
+      <c r="D11">
+        <v>-62.8</v>
+      </c>
+      <c r="E11">
+        <v>-122.33</v>
+      </c>
+      <c r="F11">
+        <v>-181.92</v>
+      </c>
+      <c r="G11">
+        <v>-199.98</v>
+      </c>
+      <c r="H11">
+        <v>-236.04</v>
+      </c>
+      <c r="I11">
+        <v>-263.88</v>
+      </c>
+      <c r="J11">
+        <v>-313.45999999999998</v>
+      </c>
+      <c r="K11">
+        <v>-358.06</v>
+      </c>
+      <c r="L11">
+        <v>-473.07</v>
+      </c>
+      <c r="M11">
+        <v>-455.16</v>
+      </c>
+      <c r="N11">
+        <v>-1129.9000000000001</v>
+      </c>
+      <c r="O11">
+        <v>-1448.84</v>
+      </c>
+      <c r="P11">
+        <v>-1605.38</v>
+      </c>
+      <c r="Q11">
+        <v>-1742.42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12">
+        <v>-72.180000000000007</v>
+      </c>
+      <c r="C12">
+        <v>-73.97</v>
+      </c>
+      <c r="D12">
+        <v>-90.68</v>
+      </c>
+      <c r="E12">
+        <v>-158.4</v>
+      </c>
+      <c r="F12">
+        <v>-241.49</v>
+      </c>
+      <c r="G12">
+        <v>-236.79</v>
+      </c>
+      <c r="H12">
+        <v>-237.05</v>
+      </c>
+      <c r="I12">
+        <v>-256.12</v>
+      </c>
+      <c r="J12">
+        <v>-360.78</v>
+      </c>
+      <c r="K12">
+        <v>-410.22</v>
+      </c>
+      <c r="L12">
+        <v>-470.08</v>
+      </c>
+      <c r="M12">
+        <v>-557.5</v>
+      </c>
+      <c r="N12">
+        <v>-1169.22</v>
+      </c>
+      <c r="O12">
+        <v>-1438.98</v>
+      </c>
+      <c r="P12">
+        <v>-1574.6</v>
+      </c>
+      <c r="Q12">
+        <v>-1668.03</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14">
+        <v>3</v>
+      </c>
+      <c r="E14">
+        <v>4</v>
+      </c>
+      <c r="F14">
+        <v>5</v>
+      </c>
+      <c r="G14">
+        <v>6</v>
+      </c>
+      <c r="H14">
+        <v>7</v>
+      </c>
+      <c r="I14">
+        <v>8</v>
+      </c>
+      <c r="J14">
+        <v>9.81</v>
+      </c>
+      <c r="K14">
+        <v>11</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+      <c r="M14">
+        <v>13</v>
+      </c>
+      <c r="N14">
+        <v>14</v>
+      </c>
+      <c r="O14">
+        <v>15</v>
+      </c>
+      <c r="P14">
+        <v>16</v>
+      </c>
+      <c r="Q14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <f>MEDIAN(B1:B12)</f>
+        <v>-80.944999999999993</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:Q15" si="0">MEDIAN(C1:C12)</f>
+        <v>-78.33</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-90.335000000000008</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="0"/>
+        <v>-207.785</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="0"/>
+        <v>-219.01</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="0"/>
+        <v>-238.595</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="0"/>
+        <v>-278.23</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>-317.53999999999996</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>-359.07</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="0"/>
+        <v>-424.98500000000001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>-478.76</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="0"/>
+        <v>-559.53500000000008</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="0"/>
+        <v>-1045.5150000000001</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="0"/>
+        <v>-1393.3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="0"/>
+        <v>-1584.2950000000001</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="0"/>
+        <v>-1706.6849999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>